<commit_message>
The date class can now handle incomplete dates and can determine if a date is valid of not.
</commit_message>
<xml_diff>
--- a/TeamHunterLeoNickReport.xlsx
+++ b/TeamHunterLeoNickReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr date1904="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leoou\OneDrive\Desktop\gedcom\GEDCOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6EB8D68-903B-4F72-9C3D-81E5B39987D6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A03C4E52-885D-41BE-942B-A65C94341135}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="130">
   <si>
     <t>Initials</t>
   </si>
@@ -438,7 +438,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="168" formatCode="m/d;@"/>
+    <numFmt numFmtId="166" formatCode="m/d;@"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -505,7 +505,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
@@ -530,7 +529,8 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -950,10 +950,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Burndown!$A$2:$A$6</c:f>
+              <c:f>Burndown!$A$2:$A$5</c:f>
               <c:numCache>
                 <c:formatCode>m/d</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>42053</c:v>
                 </c:pt>
@@ -961,17 +961,17 @@
                   <c:v>42061</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42068</c:v>
+                  <c:v>42089</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Burndown!$B$2:$B$6</c:f>
+              <c:f>Burndown!$B$2:$B$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>24</c:v>
                 </c:pt>
@@ -1735,13 +1735,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>75240</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>160920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>397800</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>25560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2123,7 +2123,7 @@
       <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -2175,7 +2175,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -2283,7 +2283,7 @@
       <c r="C6" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E6" t="s">
@@ -2300,7 +2300,7 @@
       <c r="C7" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E7" t="s">
@@ -2321,7 +2321,7 @@
         <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>29</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -2338,7 +2338,7 @@
         <v>5</v>
       </c>
       <c r="E9" t="s">
-        <v>29</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -2355,7 +2355,7 @@
         <v>10</v>
       </c>
       <c r="E10" t="s">
-        <v>29</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -2372,7 +2372,7 @@
         <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>29</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -2389,14 +2389,14 @@
         <v>15</v>
       </c>
       <c r="E12" t="s">
-        <v>29</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" t="s">
         <v>84</v>
       </c>
       <c r="C13" t="s">
@@ -2406,7 +2406,7 @@
         <v>15</v>
       </c>
       <c r="E13" t="s">
-        <v>29</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -2419,48 +2419,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" style="4" customWidth="1"/>
     <col min="2" max="2" width="9.453125" customWidth="1"/>
     <col min="3" max="3" width="15.81640625" customWidth="1"/>
     <col min="4" max="4" width="12.36328125" customWidth="1"/>
     <col min="5" max="5" width="6.81640625" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="5" customWidth="1"/>
     <col min="7" max="1025" width="10.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2468,7 +2468,7 @@
       <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="6" t="s">
         <v>46</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -2483,122 +2483,122 @@
       <c r="F14" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="G14" s="7" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15" s="8">
         <v>41065</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15" s="9">
         <v>24</v>
       </c>
-      <c r="E15" s="10">
+      <c r="E15" s="9">
         <v>0</v>
       </c>
-      <c r="F15" s="10"/>
-      <c r="G15" s="6"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="5"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B16" s="9">
+      <c r="B16" s="8">
         <v>41078</v>
       </c>
-      <c r="C16" s="10">
+      <c r="C16" s="9">
         <v>18</v>
       </c>
       <c r="D16">
         <f>C15-C16</f>
         <v>6</v>
       </c>
-      <c r="E16" s="10">
+      <c r="E16" s="9">
         <v>250</v>
       </c>
-      <c r="F16" s="10">
+      <c r="F16" s="9">
         <v>120</v>
       </c>
-      <c r="G16" s="6">
+      <c r="G16" s="5">
         <f>(E16-E15)/F16*60</f>
         <v>125.00000000000001</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B17" s="9">
+      <c r="B17" s="8">
         <v>41092</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C17" s="9">
         <v>12</v>
       </c>
       <c r="D17">
         <f>C16-C17</f>
         <v>6</v>
       </c>
-      <c r="E17" s="10">
+      <c r="E17" s="9">
         <v>480</v>
       </c>
-      <c r="F17" s="11">
+      <c r="F17" s="10">
         <v>135</v>
       </c>
-      <c r="G17" s="6">
+      <c r="G17" s="5">
         <f>(E17-E16)/F17*60</f>
         <v>102.22222222222223</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B18" s="9">
+      <c r="B18" s="8">
         <v>41106</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="9">
         <v>6</v>
       </c>
       <c r="D18">
         <f>C17-C18</f>
         <v>6</v>
       </c>
-      <c r="E18" s="10">
+      <c r="E18" s="9">
         <v>740</v>
       </c>
-      <c r="F18" s="11">
+      <c r="F18" s="10">
         <v>160</v>
       </c>
-      <c r="G18" s="6">
+      <c r="G18" s="5">
         <f>(E18-E17)/F18*60</f>
         <v>97.5</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B19" s="9">
+      <c r="B19" s="8">
         <v>41120</v>
       </c>
-      <c r="C19" s="10">
+      <c r="C19" s="9">
         <v>0</v>
       </c>
       <c r="D19">
         <f>C18-C19</f>
         <v>6</v>
       </c>
-      <c r="E19" s="10">
+      <c r="E19" s="9">
         <v>1100</v>
       </c>
-      <c r="F19" s="11">
+      <c r="F19" s="10">
         <v>145</v>
       </c>
-      <c r="G19" s="6">
+      <c r="G19" s="5">
         <f>(E19-E18)/F19*60</f>
         <v>148.9655172413793</v>
       </c>
@@ -2615,22 +2615,22 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" style="4" customWidth="1"/>
     <col min="2" max="2" width="16.6328125" customWidth="1"/>
     <col min="3" max="3" width="12.453125" customWidth="1"/>
     <col min="4" max="4" width="7.1796875" customWidth="1"/>
     <col min="5" max="5" width="6.81640625" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="5" customWidth="1"/>
     <col min="7" max="1025" width="10.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>46</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -2645,12 +2645,12 @@
       <c r="E1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="5">
+      <c r="A2" s="4">
         <v>42053</v>
       </c>
       <c r="B2">
@@ -2661,7 +2661,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="5">
+      <c r="A3" s="4">
         <v>42061</v>
       </c>
       <c r="B3">
@@ -2676,20 +2676,30 @@
       <c r="E3">
         <v>180</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="5">
         <f>D3/(E3/60)</f>
         <v>158.33333333333334</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="5">
-        <v>42068</v>
+      <c r="A4" s="4">
+        <v>42089</v>
       </c>
       <c r="B4">
         <v>12</v>
       </c>
       <c r="C4">
         <v>6</v>
+      </c>
+      <c r="D4">
+        <v>559</v>
+      </c>
+      <c r="E4">
+        <v>270</v>
+      </c>
+      <c r="F4" s="5">
+        <f>D4/(E4/60)</f>
+        <v>124.22222222222223</v>
       </c>
     </row>
   </sheetData>
@@ -2704,20 +2714,20 @@
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="K1" sqref="K1:L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.6328125" customWidth="1"/>
-    <col min="2" max="2" width="24.453125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="24.453125" style="11" customWidth="1"/>
     <col min="3" max="3" width="6.6328125" customWidth="1"/>
     <col min="4" max="4" width="10.453125" customWidth="1"/>
     <col min="5" max="5" width="6.81640625" customWidth="1"/>
     <col min="6" max="6" width="7.453125" customWidth="1"/>
     <col min="7" max="7" width="6.6328125" customWidth="1"/>
     <col min="8" max="8" width="7.6328125" customWidth="1"/>
-    <col min="9" max="9" width="10.81640625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="10.81640625" style="4" customWidth="1"/>
     <col min="10" max="10" width="10.453125" customWidth="1"/>
     <col min="11" max="11" width="38.1796875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19.26953125" bestFit="1" customWidth="1"/>
@@ -2728,7 +2738,7 @@
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -2737,25 +2747,25 @@
       <c r="D1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="K1" s="16" t="s">
+      <c r="K1" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="L1" s="16" t="s">
+      <c r="L1" s="15" t="s">
         <v>121</v>
       </c>
     </row>
@@ -2784,13 +2794,13 @@
       <c r="H2">
         <v>30</v>
       </c>
-      <c r="I2" s="5">
+      <c r="I2" s="4">
         <v>42061</v>
       </c>
-      <c r="K2" s="17" t="s">
+      <c r="K2" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="L2" s="17" t="s">
+      <c r="L2" s="16" t="s">
         <v>124</v>
       </c>
     </row>
@@ -2819,13 +2829,13 @@
       <c r="H3">
         <v>30</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="4">
         <v>42061</v>
       </c>
-      <c r="K3" s="17" t="s">
+      <c r="K3" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="L3" s="17" t="s">
+      <c r="L3" s="16" t="s">
         <v>125</v>
       </c>
     </row>
@@ -2854,7 +2864,7 @@
       <c r="H4">
         <v>30</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="4">
         <v>42061</v>
       </c>
     </row>
@@ -2883,7 +2893,7 @@
       <c r="H5">
         <v>30</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="4">
         <v>42061</v>
       </c>
     </row>
@@ -2894,7 +2904,7 @@
       <c r="B6" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D6" t="s">
@@ -2912,7 +2922,7 @@
       <c r="H6">
         <v>30</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="4">
         <v>42061</v>
       </c>
     </row>
@@ -2923,7 +2933,7 @@
       <c r="B7" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D7" t="s">
@@ -2941,7 +2951,7 @@
       <c r="H7">
         <v>30</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7" s="4">
         <v>42061</v>
       </c>
     </row>
@@ -2953,24 +2963,26 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.453125" customWidth="1"/>
     <col min="2" max="2" width="26.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="1025" width="10.453125" customWidth="1"/>
+    <col min="3" max="10" width="10.453125" customWidth="1"/>
+    <col min="11" max="11" width="38.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="1025" width="10.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -2979,23 +2991,29 @@
       <c r="D1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="13" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K1" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="L1" s="15" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>69</v>
       </c>
@@ -3006,7 +3024,7 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
+        <v>119</v>
       </c>
       <c r="E2">
         <v>100</v>
@@ -3014,12 +3032,23 @@
       <c r="F2">
         <v>60</v>
       </c>
-      <c r="G2" s="5"/>
-      <c r="I2" s="18">
-        <v>42068</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G2" s="18">
+        <v>100</v>
+      </c>
+      <c r="H2">
+        <v>30</v>
+      </c>
+      <c r="I2" s="17">
+        <v>42089</v>
+      </c>
+      <c r="K2" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="L2" s="16" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>72</v>
       </c>
@@ -3030,7 +3059,7 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>29</v>
+        <v>119</v>
       </c>
       <c r="E3">
         <v>100</v>
@@ -3038,12 +3067,21 @@
       <c r="F3">
         <v>60</v>
       </c>
-      <c r="G3" s="5"/>
-      <c r="I3" s="18">
-        <v>42068</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G3" s="18">
+        <v>100</v>
+      </c>
+      <c r="H3">
+        <v>30</v>
+      </c>
+      <c r="I3" s="17">
+        <v>42089</v>
+      </c>
+      <c r="K3" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="L3" s="16"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>75</v>
       </c>
@@ -3054,7 +3092,7 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>119</v>
       </c>
       <c r="E4">
         <v>100</v>
@@ -3062,12 +3100,17 @@
       <c r="F4">
         <v>60</v>
       </c>
-      <c r="G4" s="5"/>
-      <c r="I4" s="18">
-        <v>42068</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G4" s="18">
+        <v>100</v>
+      </c>
+      <c r="H4">
+        <v>30</v>
+      </c>
+      <c r="I4" s="17">
+        <v>42089</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>78</v>
       </c>
@@ -3078,7 +3121,7 @@
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>119</v>
       </c>
       <c r="E5">
         <v>100</v>
@@ -3086,23 +3129,28 @@
       <c r="F5">
         <v>60</v>
       </c>
-      <c r="G5" s="5"/>
-      <c r="I5" s="18">
-        <v>42068</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="G5" s="18">
+        <v>100</v>
+      </c>
+      <c r="H5">
+        <v>90</v>
+      </c>
+      <c r="I5" s="17">
+        <v>42089</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>81</v>
       </c>
       <c r="B6" t="s">
         <v>82</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>119</v>
       </c>
       <c r="E6">
         <v>100</v>
@@ -3110,23 +3158,28 @@
       <c r="F6">
         <v>60</v>
       </c>
-      <c r="G6" s="5"/>
-      <c r="I6" s="18">
-        <v>42068</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="G6" s="18">
+        <v>100</v>
+      </c>
+      <c r="H6">
+        <v>45</v>
+      </c>
+      <c r="I6" s="17">
+        <v>42089</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>84</v>
       </c>
       <c r="B7" t="s">
         <v>85</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>119</v>
       </c>
       <c r="E7">
         <v>100</v>
@@ -3134,9 +3187,14 @@
       <c r="F7">
         <v>60</v>
       </c>
-      <c r="G7" s="5"/>
-      <c r="I7" s="18">
-        <v>42068</v>
+      <c r="G7" s="18">
+        <v>100</v>
+      </c>
+      <c r="H7">
+        <v>45</v>
+      </c>
+      <c r="I7" s="17">
+        <v>42089</v>
       </c>
     </row>
   </sheetData>
@@ -3147,22 +3205,24 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1025" width="10.453125" customWidth="1"/>
+    <col min="1" max="1" width="10.453125" customWidth="1"/>
+    <col min="2" max="2" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -3171,20 +3231,140 @@
       <c r="D1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="13" t="s">
         <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>119</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+      <c r="F4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>119</v>
+      </c>
+      <c r="E5">
+        <v>10</v>
+      </c>
+      <c r="F5">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6">
+        <v>10</v>
+      </c>
+      <c r="F6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7">
+        <v>10</v>
+      </c>
+      <c r="F7">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -3210,7 +3390,7 @@
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -3219,19 +3399,19 @@
       <c r="D1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="13" t="s">
         <v>61</v>
       </c>
     </row>
@@ -3246,14 +3426,14 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.453125" customWidth="1"/>
     <col min="2" max="2" width="28.1796875" customWidth="1"/>
-    <col min="3" max="3" width="49.453125" style="12" customWidth="1"/>
+    <col min="3" max="3" width="49.453125" style="11" customWidth="1"/>
     <col min="4" max="1025" width="10.453125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3264,7 +3444,7 @@
       <c r="B1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>62</v>
       </c>
     </row>
@@ -3275,7 +3455,7 @@
       <c r="B2" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>63</v>
       </c>
     </row>
@@ -3286,7 +3466,7 @@
       <c r="B3" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>64</v>
       </c>
     </row>
@@ -3297,7 +3477,7 @@
       <c r="B4" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>65</v>
       </c>
     </row>
@@ -3308,7 +3488,7 @@
       <c r="B5" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>66</v>
       </c>
     </row>
@@ -3319,7 +3499,7 @@
       <c r="B6" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>67</v>
       </c>
     </row>
@@ -3330,7 +3510,7 @@
       <c r="B7" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>68</v>
       </c>
     </row>
@@ -3341,7 +3521,7 @@
       <c r="B8" t="s">
         <v>70</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>71</v>
       </c>
     </row>
@@ -3352,7 +3532,7 @@
       <c r="B9" t="s">
         <v>73</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>74</v>
       </c>
     </row>
@@ -3363,7 +3543,7 @@
       <c r="B10" t="s">
         <v>76</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>77</v>
       </c>
     </row>
@@ -3374,7 +3554,7 @@
       <c r="B11" t="s">
         <v>79</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>80</v>
       </c>
     </row>
@@ -3385,62 +3565,62 @@
       <c r="B12" t="s">
         <v>82</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
+      <c r="A13" t="s">
         <v>84</v>
       </c>
       <c r="B13" t="s">
         <v>85</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="3" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+      <c r="A14" t="s">
         <v>87</v>
       </c>
       <c r="B14" t="s">
         <v>88</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
+      <c r="A15" t="s">
         <v>90</v>
       </c>
       <c r="B15" t="s">
         <v>91</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+      <c r="A16" t="s">
         <v>92</v>
       </c>
       <c r="B16" t="s">
         <v>93</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
+      <c r="A17" t="s">
         <v>94</v>
       </c>
       <c r="B17" t="s">
         <v>95</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>129</v>
       </c>
     </row>
@@ -3451,7 +3631,7 @@
       <c r="B18" t="s">
         <v>97</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>89</v>
       </c>
     </row>
@@ -3462,7 +3642,7 @@
       <c r="B19" t="s">
         <v>99</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="3" t="s">
         <v>100</v>
       </c>
     </row>
@@ -3473,7 +3653,7 @@
       <c r="B20" t="s">
         <v>102</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="3" t="s">
         <v>103</v>
       </c>
     </row>
@@ -3484,7 +3664,7 @@
       <c r="B21" t="s">
         <v>105</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="3" t="s">
         <v>106</v>
       </c>
     </row>
@@ -3495,7 +3675,7 @@
       <c r="B22" t="s">
         <v>108</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="3" t="s">
         <v>109</v>
       </c>
     </row>
@@ -3506,7 +3686,7 @@
       <c r="B23" t="s">
         <v>111</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="3" t="s">
         <v>112</v>
       </c>
     </row>
@@ -3517,7 +3697,7 @@
       <c r="B24" t="s">
         <v>114</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="3" t="s">
         <v>115</v>
       </c>
     </row>
@@ -3528,7 +3708,7 @@
       <c r="B25" t="s">
         <v>117</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="3" t="s">
         <v>118</v>
       </c>
     </row>

</xml_diff>